<commit_message>
Working Get with GUI
</commit_message>
<xml_diff>
--- a/log-statistics.xlsx
+++ b/log-statistics.xlsx
@@ -96,7 +96,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>210.0</v>
+        <v>171.0</v>
       </c>
     </row>
     <row r="3">
@@ -104,7 +104,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>210.0</v>
+        <v>171.0</v>
       </c>
     </row>
     <row r="4">
@@ -112,7 +112,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>76.0</v>
+        <v>17.0</v>
       </c>
     </row>
     <row r="5">
@@ -120,7 +120,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>19.0</v>
+        <v>67.0</v>
       </c>
     </row>
     <row r="6">
@@ -128,7 +128,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>17.0</v>
+        <v>48.0</v>
       </c>
     </row>
     <row r="7">
@@ -136,7 +136,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>70.0</v>
+        <v>10.0</v>
       </c>
     </row>
     <row r="8">
@@ -144,7 +144,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>28.0</v>
+        <v>29.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed how datas are stored in stats
</commit_message>
<xml_diff>
--- a/log-statistics.xlsx
+++ b/log-statistics.xlsx
@@ -14,7 +14,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
-    <t>2019-06-1</t>
+    <t>2019-06-15</t>
   </si>
   <si>
     <t>RandomLogs</t>
@@ -23,19 +23,19 @@
     <t>main</t>
   </si>
   <si>
-    <t>0</t>
+    <t>ERROR</t>
   </si>
   <si>
-    <t>1</t>
+    <t>INFO</t>
   </si>
   <si>
-    <t>2</t>
+    <t>DEBUG</t>
   </si>
   <si>
-    <t>3</t>
+    <t>FATAL</t>
   </si>
   <si>
-    <t>4</t>
+    <t>WARN</t>
   </si>
 </sst>
 </file>
@@ -84,7 +84,7 @@
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="100"/>
   <sheetData>
     <row r="1">
       <c r="B1" t="s">
@@ -96,7 +96,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>171.0</v>
+        <v>25.0</v>
       </c>
     </row>
     <row r="3">
@@ -104,7 +104,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>171.0</v>
+        <v>25.0</v>
       </c>
     </row>
     <row r="4">
@@ -112,7 +112,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>17.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="5">
@@ -120,7 +120,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>67.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="6">
@@ -128,7 +128,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>48.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="7">
@@ -136,7 +136,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>10.0</v>
+        <v>7.0</v>
       </c>
     </row>
     <row r="8">
@@ -144,7 +144,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>29.0</v>
+        <v>10.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
made doget for stats send excel content to client instead of downloading at server side
</commit_message>
<xml_diff>
--- a/log-statistics.xlsx
+++ b/log-statistics.xlsx
@@ -14,7 +14,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
-    <t>2019-06-15</t>
+    <t>2019-06-16</t>
   </si>
   <si>
     <t>RandomLogs</t>
@@ -84,7 +84,7 @@
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="100"/>
+  <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
       <c r="B1" t="s">
@@ -96,7 +96,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>25.0</v>
+        <v>90.0</v>
       </c>
     </row>
     <row r="3">
@@ -104,7 +104,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>25.0</v>
+        <v>90.0</v>
       </c>
     </row>
     <row r="4">
@@ -112,7 +112,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>3.0</v>
+        <v>16.0</v>
       </c>
     </row>
     <row r="5">
@@ -120,7 +120,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>3.0</v>
+        <v>13.0</v>
       </c>
     </row>
     <row r="6">
@@ -128,7 +128,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>2.0</v>
+        <v>17.0</v>
       </c>
     </row>
     <row r="7">
@@ -136,7 +136,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>7.0</v>
+        <v>23.0</v>
       </c>
     </row>
     <row r="8">
@@ -144,7 +144,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>10.0</v>
+        <v>21.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
implemented executable jars and jaCoCo
</commit_message>
<xml_diff>
--- a/log-statistics.xlsx
+++ b/log-statistics.xlsx
@@ -17,10 +17,10 @@
     <t>2019-06-16</t>
   </si>
   <si>
-    <t>RandomLogs</t>
+    <t>testlogger</t>
   </si>
   <si>
-    <t>main</t>
+    <t>testing</t>
   </si>
   <si>
     <t>ERROR</t>
@@ -29,10 +29,10 @@
     <t>INFO</t>
   </si>
   <si>
-    <t>DEBUG</t>
+    <t>FATAL</t>
   </si>
   <si>
-    <t>FATAL</t>
+    <t>DEBUG</t>
   </si>
   <si>
     <t>WARN</t>
@@ -96,7 +96,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>90.0</v>
+        <v>30.0</v>
       </c>
     </row>
     <row r="3">
@@ -104,7 +104,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>90.0</v>
+        <v>30.0</v>
       </c>
     </row>
     <row r="4">
@@ -112,7 +112,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>16.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="5">
@@ -120,7 +120,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>13.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="6">
@@ -128,7 +128,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>17.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="7">
@@ -136,7 +136,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>23.0</v>
+        <v>6.0</v>
       </c>
     </row>
     <row r="8">
@@ -144,7 +144,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>21.0</v>
+        <v>6.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>